<commit_message>
feat: energy sensitivity boxplots calculated
</commit_message>
<xml_diff>
--- a/data/LEAP_Supply_Emissions.xlsx
+++ b/data/LEAP_Supply_Emissions.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giann\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ev\Documents\Software Projects\SDSN GCH\ScenViz_Template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191D5E59-D490-4C07-893D-53AF44BE292F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE4428-A9C4-46F7-A8A3-B80A6C9057C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01BF1780-3214-47DB-9C17-C2F5550468A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{01BF1780-3214-47DB-9C17-C2F5550468A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sensitivity" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,8 +95,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;&quot;\-&quot;&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;&quot;\-&quot;&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -146,14 +146,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -491,23 +491,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F58F65-D173-4C9B-B57C-646E19A136BF}">
   <dimension ref="A1:I320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -528,7 +528,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2022</v>
       </c>
@@ -549,7 +549,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2023</v>
       </c>
@@ -570,7 +570,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2024</v>
       </c>
@@ -591,7 +591,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2025</v>
       </c>
@@ -612,7 +612,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2026</v>
       </c>
@@ -633,7 +633,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2027</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2028</v>
       </c>
@@ -675,7 +675,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2029</v>
       </c>
@@ -696,7 +696,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2030</v>
       </c>
@@ -717,7 +717,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2031</v>
       </c>
@@ -738,7 +738,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2032</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2033</v>
       </c>
@@ -780,7 +780,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2034</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2035</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2036</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2037</v>
       </c>
@@ -864,7 +864,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2038</v>
       </c>
@@ -885,7 +885,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2039</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2040</v>
       </c>
@@ -927,7 +927,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2041</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2042</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2043</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2044</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2045</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2046</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2047</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2048</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2049</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2050</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2022</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2024</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2025</v>
       </c>
@@ -1221,7 +1221,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2026</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2027</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2028</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2029</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2030</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2031</v>
       </c>
@@ -1347,7 +1347,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2032</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2033</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2034</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2035</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2036</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2037</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2038</v>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2039</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2040</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2041</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2042</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2043</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2044</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2045</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2046</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2047</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2048</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2049</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2050</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2022</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2024</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2025</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2026</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2027</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2028</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2029</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2030</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2031</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2032</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2033</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2034</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2035</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2036</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2037</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2038</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2039</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2040</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2041</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2042</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2043</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>2044</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2045</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2046</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2047</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>2048</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>2049</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>2050</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>2022</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2023</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2024</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2025</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2026</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2027</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2028</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>2029</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2030</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2031</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2032</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2033</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2034</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2035</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2036</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2037</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2038</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2039</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2040</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2041</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2042</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2043</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2044</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2045</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2046</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2047</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2048</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2049</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2050</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2022</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2023</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2024</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2025</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2026</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2027</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2028</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2029</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2030</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2031</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2032</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2033</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2034</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2035</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2036</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2037</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2038</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2039</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2040</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2041</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2042</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2043</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2044</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2045</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2046</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2047</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2048</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2049</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2050</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2022</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2023</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2024</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2025</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2026</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2027</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>2028</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>2029</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2030</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>2031</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>2032</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>2033</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>2034</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>2035</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2036</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2037</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2038</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2039</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2040</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2041</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2042</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2043</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2044</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2045</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2046</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2047</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2048</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2049</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2050</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2022</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2023</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2024</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2025</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2026</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2027</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2028</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2029</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2030</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2031</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2032</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2033</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2034</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2035</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2036</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2037</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2038</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2039</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2040</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2041</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2042</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2043</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2044</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2045</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2046</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2047</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2048</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2049</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>2050</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>2022</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>2023</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>2024</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>2025</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>2026</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>2027</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>2028</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>2029</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>2030</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>2031</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>2032</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2033</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>2034</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>2035</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>2036</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>2037</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>2038</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>2039</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>2040</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>2041</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>2042</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>2043</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>2044</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>2045</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>2046</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>2047</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>2048</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>2049</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>2050</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>2022</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>2023</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>2024</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>2025</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>2026</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>2027</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>2028</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>2029</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>2030</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>2031</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>2032</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>2033</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>2034</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>2035</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>2036</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>2037</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>2038</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>2039</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>2040</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>2041</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>2042</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>2043</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>2044</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>2045</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>2046</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>2047</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>2048</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>2049</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>2050</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>2022</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>2023</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>2024</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>2025</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>2026</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>2027</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>2028</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>2029</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>2030</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>2031</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>2032</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>2033</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>2034</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>2035</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>2036</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>2037</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>2038</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>2039</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>2040</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>2041</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>2042</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>2043</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>2044</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>2045</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>2046</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>2047</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>2048</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>2049</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>2050</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>2022</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>2023</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>2024</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>2025</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>2026</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>2027</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>2028</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>2029</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>2030</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>2031</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>2032</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>2033</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>2034</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>2035</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>2036</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>2037</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>2038</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>2039</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>2040</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>2041</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>2042</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>2043</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>2044</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>2045</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>2046</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>2047</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>2048</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>2049</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>2050</v>
       </c>
@@ -6192,13 +6192,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD679B95-863C-438C-841F-851E5A114106}">
   <dimension ref="A1:AD75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -6598,7 +6598,7 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6630,7 +6630,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -7030,7 +7030,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -7062,7 +7062,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -7094,7 +7094,7 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -7126,7 +7126,7 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2022</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2024</v>
       </c>
@@ -7223,7 +7223,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2025</v>
       </c>
@@ -7244,7 +7244,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2026</v>
       </c>
@@ -7265,7 +7265,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2027</v>
       </c>
@@ -7286,7 +7286,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2028</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2029</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2030</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2031</v>
       </c>
@@ -7370,7 +7370,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2032</v>
       </c>
@@ -7391,7 +7391,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2033</v>
       </c>
@@ -7412,7 +7412,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2034</v>
       </c>
@@ -7433,7 +7433,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2035</v>
       </c>
@@ -7454,7 +7454,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2036</v>
       </c>
@@ -7475,7 +7475,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2037</v>
       </c>
@@ -7496,7 +7496,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2038</v>
       </c>
@@ -7517,7 +7517,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2039</v>
       </c>
@@ -7538,7 +7538,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2040</v>
       </c>
@@ -7559,7 +7559,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2041</v>
       </c>
@@ -7580,7 +7580,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2042</v>
       </c>
@@ -7601,7 +7601,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2043</v>
       </c>
@@ -7622,7 +7622,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2044</v>
       </c>
@@ -7643,7 +7643,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2045</v>
       </c>
@@ -7664,7 +7664,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2046</v>
       </c>
@@ -7685,7 +7685,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2047</v>
       </c>
@@ -7706,7 +7706,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2048</v>
       </c>
@@ -7727,7 +7727,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2049</v>
       </c>
@@ -7748,7 +7748,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2050</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2022</v>
       </c>
@@ -7790,7 +7790,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -7811,7 +7811,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2024</v>
       </c>
@@ -7832,7 +7832,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2025</v>
       </c>
@@ -7853,7 +7853,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2026</v>
       </c>
@@ -7874,7 +7874,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2027</v>
       </c>
@@ -7895,7 +7895,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2028</v>
       </c>
@@ -7916,7 +7916,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2029</v>
       </c>
@@ -7937,7 +7937,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2030</v>
       </c>
@@ -7958,7 +7958,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2031</v>
       </c>
@@ -7979,7 +7979,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2032</v>
       </c>
@@ -8000,7 +8000,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2033</v>
       </c>
@@ -8021,7 +8021,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2034</v>
       </c>
@@ -8042,7 +8042,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2035</v>
       </c>
@@ -8063,7 +8063,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2036</v>
       </c>
@@ -8084,7 +8084,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2037</v>
       </c>
@@ -8105,7 +8105,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2038</v>
       </c>
@@ -8126,7 +8126,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2039</v>
       </c>
@@ -8147,7 +8147,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2040</v>
       </c>
@@ -8168,7 +8168,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2041</v>
       </c>
@@ -8189,7 +8189,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2042</v>
       </c>
@@ -8210,7 +8210,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2043</v>
       </c>
@@ -8231,7 +8231,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2044</v>
       </c>
@@ -8252,7 +8252,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2045</v>
       </c>
@@ -8273,7 +8273,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2046</v>
       </c>
@@ -8294,7 +8294,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2047</v>
       </c>
@@ -8315,7 +8315,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2048</v>
       </c>
@@ -8336,7 +8336,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2049</v>
       </c>
@@ -8357,7 +8357,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2050</v>
       </c>
@@ -8378,7 +8378,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -8389,7 +8389,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>

</xml_diff>